<commit_message>
- Modified login_key column name to login_pwd. - Modified group-config script.
</commit_message>
<xml_diff>
--- a/group-config.xlsx
+++ b/group-config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="groups" sheetId="2" r:id="rId1"/>
@@ -488,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
- Updated email notification parameters. - Restructured group-config to a single file - Added student-config feature
</commit_message>
<xml_diff>
--- a/group-config.xlsx
+++ b/group-config.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="42">
   <si>
     <t>Group_Name</t>
   </si>
@@ -120,6 +120,27 @@
   </si>
   <si>
     <t>A13</t>
+  </si>
+  <si>
+    <t>STUDENT_ID</t>
+  </si>
+  <si>
+    <t>IS_MANAGER</t>
+  </si>
+  <si>
+    <t>team1</t>
+  </si>
+  <si>
+    <t>team2</t>
+  </si>
+  <si>
+    <t>team3</t>
+  </si>
+  <si>
+    <t>team4</t>
+  </si>
+  <si>
+    <t>team5</t>
   </si>
 </sst>
 </file>
@@ -486,21 +507,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A6"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -508,13 +531,19 @@
         <v>31</v>
       </c>
       <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
         <v>32</v>
       </c>
-      <c r="D1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -522,13 +551,16 @@
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -536,13 +568,16 @@
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -550,13 +585,16 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -564,13 +602,19 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -578,10 +622,314 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>37</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>13</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>13</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>13</v>
+      </c>
+      <c r="C21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>13</v>
+      </c>
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>13</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -594,7 +942,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>